<commit_message>
initial change - more modification needed soon
</commit_message>
<xml_diff>
--- a/server/excel_controller/config/vn/cell-style-samples.xlsx
+++ b/server/excel_controller/config/vn/cell-style-samples.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MayRentManagement\server\excel_controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MayRentManagement\server\excel_controller\config\vn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,31 +21,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t xml:space="preserve"> Text</t>
+    <t>Ghép</t>
   </si>
   <si>
-    <t xml:space="preserve"> Number</t>
+    <t>Tiêu đề hướng dẫn</t>
   </si>
   <si>
-    <t xml:space="preserve"> Binary</t>
+    <t>Hướng dẫn</t>
   </si>
   <si>
-    <t xml:space="preserve"> Number (m2)</t>
+    <t>Nhị phân</t>
   </si>
   <si>
-    <t>Instruction Title</t>
+    <t>Ngày</t>
   </si>
   <si>
-    <t>Merge</t>
+    <t>Mã số</t>
   </si>
   <si>
-    <t>Instruction Text</t>
+    <t>Diện tích</t>
   </si>
   <si>
-    <t xml:space="preserve"> Date</t>
+    <t>Số</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>Chữ</t>
   </si>
 </sst>
 </file>
@@ -934,7 +934,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,31 +946,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>